<commit_message>
changes in home page
</commit_message>
<xml_diff>
--- a/data/contacts.xlsx
+++ b/data/contacts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,10 +471,8 @@
           <t>a@gmail.com</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>06206872005</t>
-        </is>
+      <c r="C2" t="n">
+        <v>6206872005</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -484,6 +482,33 @@
       <c r="E2" t="inlineStr">
         <is>
           <t>gbghfjyuikui</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>jkljkl;lk</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>isha@gmail.com</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>jjor4455654</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>sdkdklflkrk</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>jlkjlkk;k;</t>
         </is>
       </c>
     </row>

</xml_diff>